<commit_message>
Review 2: Lista de materiales
</commit_message>
<xml_diff>
--- a/docs/Lista de materiales.xlsx
+++ b/docs/Lista de materiales.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="44">
   <si>
     <t>SERIAL</t>
   </si>
@@ -134,9 +134,6 @@
     <t>2cm</t>
   </si>
   <si>
-    <t>6cm a la mitad</t>
-  </si>
-  <si>
     <t>Para fijar cables del altavoz</t>
   </si>
   <si>
@@ -161,14 +158,20 @@
     <t>Empaque final</t>
   </si>
   <si>
-    <t>Pieza de 6x0,6cm dividida en 3 piezas de 2 cm</t>
+    <t>3cm</t>
+  </si>
+  <si>
+    <t>3cm divididas en 3 piezas de 1cm cada una</t>
+  </si>
+  <si>
+    <t>REV 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -210,6 +213,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -424,7 +434,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -512,32 +522,35 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1577,7 +1590,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1592,41 +1605,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="31"/>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
+      <c r="A2" s="39"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
     </row>
-    <row r="3" spans="1:8" ht="15.75" thickBot="1"/>
+    <row r="3" spans="1:8" ht="19.5" thickBot="1">
+      <c r="F3" s="40" t="s">
+        <v>43</v>
+      </c>
+    </row>
     <row r="4" spans="1:8" ht="30.75" thickBot="1">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="37" t="s">
+      <c r="D4" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="37" t="s">
+      <c r="E4" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="39" t="s">
+      <c r="F4" s="38" t="s">
         <v>4</v>
       </c>
       <c r="G4" s="2"/>
@@ -1647,7 +1664,7 @@
         <v>1</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
@@ -1667,7 +1684,7 @@
         <v>1</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
@@ -1687,7 +1704,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
@@ -1705,7 +1722,7 @@
         <v>32</v>
       </c>
       <c r="F8" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G8" s="14"/>
       <c r="H8" s="14"/>
@@ -1720,7 +1737,7 @@
         <v>29</v>
       </c>
       <c r="E9" s="24" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="F9" s="18" t="s">
         <v>42</v>
@@ -1743,7 +1760,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G10" s="19"/>
       <c r="H10" s="19"/>
@@ -1763,7 +1780,7 @@
         <v>1</v>
       </c>
       <c r="F11" s="18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
@@ -1776,8 +1793,8 @@
       <c r="C12" s="22"/>
       <c r="D12" s="22"/>
       <c r="E12" s="30"/>
-      <c r="F12" s="32" t="s">
-        <v>36</v>
+      <c r="F12" s="31" t="s">
+        <v>35</v>
       </c>
       <c r="G12" s="23"/>
       <c r="H12" s="23"/>
@@ -1797,7 +1814,7 @@
         <v>1</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
@@ -1817,7 +1834,7 @@
         <v>1</v>
       </c>
       <c r="F14" s="16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
@@ -1837,7 +1854,7 @@
         <v>1</v>
       </c>
       <c r="F15" s="18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G15" s="19"/>
       <c r="H15" s="14"/>
@@ -1857,7 +1874,7 @@
         <v>1</v>
       </c>
       <c r="F16" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G16" s="19"/>
       <c r="H16" s="19"/>
@@ -1866,18 +1883,18 @@
       <c r="A17" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="33" t="s">
+      <c r="B17" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="33"/>
-      <c r="D17" s="34" t="s">
+      <c r="C17" s="32"/>
+      <c r="D17" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="E17" s="34">
+      <c r="E17" s="33">
         <v>1</v>
       </c>
-      <c r="F17" s="35" t="s">
-        <v>41</v>
+      <c r="F17" s="34" t="s">
+        <v>40</v>
       </c>
       <c r="G17" s="19"/>
       <c r="H17" s="14"/>
@@ -1887,7 +1904,7 @@
     <mergeCell ref="A1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>